<commit_message>
making "progress" on project 2
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mab916\Documents\Local Coding\Project 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19EE25EB-9BAC-424E-A222-B09C4E9649EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4736964-BCB0-479F-BAA8-3F8C75E513D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="3240" windowWidth="15600" windowHeight="11160" xr2:uid="{52E6B518-8B58-4230-9FD8-DAA171655137}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>time</t>
   </si>
@@ -63,6 +63,21 @@
   </si>
   <si>
     <t>mol/dL</t>
+  </si>
+  <si>
+    <t>c mol/dL</t>
+  </si>
+  <si>
+    <t>cadj mol/dL</t>
+  </si>
+  <si>
+    <t>cadj g/dL</t>
+  </si>
+  <si>
+    <t>hpadj g/dL</t>
+  </si>
+  <si>
+    <t>hpadj mol/dL</t>
   </si>
 </sst>
 </file>
@@ -414,18 +429,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1C9F794-AA0E-4C28-B2B8-93AB6B838B61}">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -441,23 +460,38 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
       <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -473,12 +507,30 @@
       <c r="E2">
         <v>0.56250000000000089</v>
       </c>
+      <c r="F2">
+        <v>-2.4374999999999947</v>
+      </c>
       <c r="G2">
-        <f>D2/(1000*64000)</f>
+        <f>F2/(100*64000)</f>
+        <v>-3.8085937499999915E-7</v>
+      </c>
+      <c r="H2">
+        <v>-2.1458333333333282</v>
+      </c>
+      <c r="I2">
+        <f>H2/(100*64000)</f>
+        <v>-3.352864583333325E-7</v>
+      </c>
+      <c r="J2">
+        <f t="shared" ref="J2:J25" si="0">D2/(1000*64000)</f>
         <v>-3.3528645833333253E-8</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K2">
+        <f t="shared" ref="K2:K25" si="1">B2/(1000*64000)</f>
+        <v>-3.808593749999992E-8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -494,12 +546,30 @@
       <c r="E3">
         <v>0.68844631841076354</v>
       </c>
+      <c r="F3">
+        <v>-4.7566333333333297</v>
+      </c>
       <c r="G3">
-        <f t="shared" ref="G3:G25" si="0">D3/(1000*64000)</f>
+        <f t="shared" ref="G3:G25" si="2">F3/(100*64000)</f>
+        <v>-7.4322395833333279E-7</v>
+      </c>
+      <c r="H3">
+        <v>-1.889933333333329</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I25" si="3">H3/(100*64000)</f>
+        <v>-2.9530208333333265E-7</v>
+      </c>
+      <c r="J3">
+        <f t="shared" si="0"/>
         <v>-2.5390624999999936E-8</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K3">
+        <f t="shared" si="1"/>
+        <v>-2.0507812499999929E-8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -515,12 +585,30 @@
       <c r="E4">
         <v>0.83229101480992329</v>
       </c>
+      <c r="F4">
+        <v>-9.2781999999999947</v>
+      </c>
       <c r="G4">
+        <f t="shared" si="2"/>
+        <v>-1.4497187499999993E-6</v>
+      </c>
+      <c r="H4">
+        <v>-2.6072999999999955</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="3"/>
+        <v>-4.073906249999993E-7</v>
+      </c>
+      <c r="J4">
         <f t="shared" si="0"/>
         <v>-2.8320312499999931E-8</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <f t="shared" si="1"/>
+        <v>-3.3203124999999907E-8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -536,12 +624,30 @@
       <c r="E5">
         <v>0.74999999999999978</v>
       </c>
+      <c r="F5">
+        <v>-13.606366666666663</v>
+      </c>
       <c r="G5">
+        <f t="shared" si="2"/>
+        <v>-2.1259947916666661E-6</v>
+      </c>
+      <c r="H5">
+        <v>-4.1729333333333267</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="3"/>
+        <v>-6.5202083333333228E-7</v>
+      </c>
+      <c r="J5">
         <f t="shared" si="0"/>
         <v>-4.0364583333333227E-8</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <f t="shared" si="1"/>
+        <v>-3.8736979166666605E-8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -557,24 +663,42 @@
       <c r="E6">
         <v>1.638167802760147</v>
       </c>
+      <c r="F6">
+        <v>-16.199466666666662</v>
+      </c>
       <c r="G6">
+        <f t="shared" si="2"/>
+        <v>-2.5311666666666662E-6</v>
+      </c>
+      <c r="H6">
+        <v>26.517333333333333</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="3"/>
+        <v>4.1433333333333332E-6</v>
+      </c>
+      <c r="J6">
         <f t="shared" si="0"/>
         <v>4.5572916666666666E-7</v>
       </c>
-      <c r="I6">
+      <c r="K6">
+        <f t="shared" si="1"/>
+        <v>-1.3020833333333254E-8</v>
+      </c>
+      <c r="L6">
         <v>0</v>
       </c>
-      <c r="J6">
+      <c r="M6">
         <v>0.83333333333332826</v>
       </c>
-      <c r="K6">
+      <c r="N6">
         <v>10</v>
       </c>
-      <c r="L6">
+      <c r="O6">
         <v>-19.166666666666668</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -590,24 +714,42 @@
       <c r="E7">
         <v>3.12833155744933</v>
       </c>
+      <c r="F7">
+        <v>25.650833333333342</v>
+      </c>
       <c r="G7">
+        <f t="shared" si="2"/>
+        <v>4.0079427083333343E-6</v>
+      </c>
+      <c r="H7">
+        <v>44.921833333333339</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="3"/>
+        <v>7.0190364583333345E-6</v>
+      </c>
+      <c r="J7">
         <f t="shared" si="0"/>
         <v>7.6399739583333334E-7</v>
       </c>
-      <c r="I7">
+      <c r="K7">
+        <f t="shared" si="1"/>
+        <v>7.1126302083333343E-7</v>
+      </c>
+      <c r="L7">
         <v>30</v>
       </c>
-      <c r="J7">
+      <c r="M7">
         <v>-15.520833333333343</v>
       </c>
-      <c r="K7">
+      <c r="N7">
         <v>30</v>
       </c>
-      <c r="L7">
+      <c r="O7">
         <v>-18.895833333333336</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -623,24 +765,42 @@
       <c r="E8">
         <v>1.1874999999999993</v>
       </c>
+      <c r="F8">
+        <v>107.4237</v>
+      </c>
       <c r="G8">
+        <f t="shared" si="2"/>
+        <v>1.6784953125E-5</v>
+      </c>
+      <c r="H8">
+        <v>32.22806666666667</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="3"/>
+        <v>5.0356354166666669E-6</v>
+      </c>
+      <c r="J8">
         <f t="shared" si="0"/>
         <v>5.9049479166666676E-7</v>
       </c>
-      <c r="I8">
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>2.0634765624999999E-6</v>
+      </c>
+      <c r="L8">
         <v>110</v>
       </c>
-      <c r="J8">
+      <c r="M8">
         <v>-22.0625</v>
       </c>
-      <c r="K8">
+      <c r="N8">
         <v>20</v>
       </c>
-      <c r="L8">
+      <c r="O8">
         <v>-17.791666666666671</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -656,24 +816,42 @@
       <c r="E9">
         <v>2.0653389552322916</v>
       </c>
+      <c r="F9">
+        <v>153.03579999999999</v>
+      </c>
       <c r="G9">
+        <f t="shared" si="2"/>
+        <v>2.3911843749999998E-5</v>
+      </c>
+      <c r="H9">
+        <v>37.186033333333341</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="3"/>
+        <v>5.8103177083333349E-6</v>
+      </c>
+      <c r="J9">
         <f t="shared" si="0"/>
         <v>6.969401041666667E-7</v>
       </c>
-      <c r="I9">
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>2.8548177083333329E-6</v>
+      </c>
+      <c r="L9">
         <v>160</v>
       </c>
-      <c r="J9">
+      <c r="M9">
         <v>-22.708333333333314</v>
       </c>
-      <c r="K9">
+      <c r="N9">
         <v>30</v>
       </c>
-      <c r="L9">
+      <c r="O9">
         <v>-14.604166666666671</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -689,24 +867,42 @@
       <c r="E10">
         <v>3.5981404340760994</v>
       </c>
+      <c r="F10">
+        <v>156.19546666666668</v>
+      </c>
       <c r="G10">
+        <f t="shared" si="2"/>
+        <v>2.4405541666666667E-5</v>
+      </c>
+      <c r="H10">
+        <v>50.420733333333345</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="3"/>
+        <v>7.8782395833333358E-6</v>
+      </c>
+      <c r="J10">
         <f t="shared" si="0"/>
         <v>9.3684895833333352E-7</v>
       </c>
-      <c r="I10">
+      <c r="K10">
+        <f t="shared" si="1"/>
+        <v>2.9869791666666666E-6</v>
+      </c>
+      <c r="L10">
         <v>180</v>
       </c>
-      <c r="J10">
+      <c r="M10">
         <v>-11.166666666666657</v>
       </c>
-      <c r="K10">
+      <c r="N10">
         <v>50</v>
       </c>
-      <c r="L10">
+      <c r="O10">
         <v>-9.9583333333333428</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -722,18 +918,36 @@
       <c r="E11">
         <v>3.4687969216045684</v>
       </c>
+      <c r="F11">
+        <v>161.31936666666667</v>
+      </c>
       <c r="G11">
+        <f t="shared" si="2"/>
+        <v>2.5206151041666667E-5</v>
+      </c>
+      <c r="H11">
+        <v>74.328000000000003</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="3"/>
+        <v>1.161375E-5</v>
+      </c>
+      <c r="J11">
         <f t="shared" si="0"/>
         <v>1.3476562499999999E-6</v>
       </c>
       <c r="K11">
+        <f t="shared" si="1"/>
+        <v>3.1539713541666667E-6</v>
+      </c>
+      <c r="N11">
         <v>70</v>
       </c>
-      <c r="L11">
+      <c r="O11">
         <v>-16.25</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -749,18 +963,36 @@
       <c r="E12">
         <v>4.376339080784307</v>
       </c>
+      <c r="F12">
+        <v>163.6575</v>
+      </c>
       <c r="G12">
+        <f t="shared" si="2"/>
+        <v>2.5571484374999999E-5</v>
+      </c>
+      <c r="H12">
+        <v>115.03283333333336</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="3"/>
+        <v>1.7973880208333336E-5</v>
+      </c>
+      <c r="J12">
         <f t="shared" si="0"/>
         <v>2.0250651041666668E-6</v>
       </c>
       <c r="K12">
+        <f t="shared" si="1"/>
+        <v>3.2815755208333337E-6</v>
+      </c>
+      <c r="N12">
         <v>120</v>
       </c>
-      <c r="L12">
+      <c r="O12">
         <v>-9.6041666666666856</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -776,18 +1008,36 @@
       <c r="E13">
         <v>5.8220128249028589</v>
       </c>
+      <c r="F13">
+        <v>162.93903333333333</v>
+      </c>
       <c r="G13">
+        <f t="shared" si="2"/>
+        <v>2.5459223958333332E-5</v>
+      </c>
+      <c r="H13">
+        <v>129.84773333333334</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="3"/>
+        <v>2.0288708333333333E-5</v>
+      </c>
+      <c r="J13">
         <f t="shared" si="0"/>
         <v>2.3020833333333337E-6</v>
       </c>
       <c r="K13">
+        <f t="shared" si="1"/>
+        <v>3.3655598958333334E-6</v>
+      </c>
+      <c r="N13">
         <v>150</v>
       </c>
-      <c r="L13">
+      <c r="O13">
         <v>2.6666666666666572</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -803,18 +1053,36 @@
       <c r="E14">
         <v>7.2043281262030305</v>
       </c>
+      <c r="F14">
+        <v>172.5598</v>
+      </c>
       <c r="G14">
+        <f t="shared" si="2"/>
+        <v>2.6962468750000001E-5</v>
+      </c>
+      <c r="H14">
+        <v>166.56436666666667</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="3"/>
+        <v>2.6025682291666669E-5</v>
+      </c>
+      <c r="J14">
         <f t="shared" si="0"/>
         <v>2.9254557291666669E-6</v>
       </c>
       <c r="K14">
+        <f t="shared" si="1"/>
+        <v>3.615234375E-6</v>
+      </c>
+      <c r="N14">
         <v>180</v>
       </c>
-      <c r="L14">
+      <c r="O14">
         <v>-7.2291666666666856</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -830,12 +1098,30 @@
       <c r="E15">
         <v>7.5537139044313903</v>
       </c>
+      <c r="F15">
+        <v>182.99896666666666</v>
+      </c>
       <c r="G15">
+        <f t="shared" si="2"/>
+        <v>2.8593588541666667E-5</v>
+      </c>
+      <c r="H15">
+        <v>167.74523333333329</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="3"/>
+        <v>2.6210192708333325E-5</v>
+      </c>
+      <c r="J15">
         <f t="shared" si="0"/>
         <v>2.9977213541666659E-6</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K15">
+        <f t="shared" si="1"/>
+        <v>3.8818359374999994E-6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -852,14 +1138,29 @@
         <v>4.3419885517275691</v>
       </c>
       <c r="F16">
-        <v>249.95833333333331</v>
+        <v>177.63153333333332</v>
       </c>
       <c r="G16">
+        <f t="shared" si="2"/>
+        <v>2.7754927083333332E-5</v>
+      </c>
+      <c r="H16">
+        <v>184.18200000000002</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="3"/>
+        <v>2.8778437500000001E-5</v>
+      </c>
+      <c r="J16">
         <f t="shared" si="0"/>
         <v>3.3125E-6</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K16">
+        <f t="shared" si="1"/>
+        <v>3.905598958333333E-6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -876,14 +1177,29 @@
         <v>8.3839349104900212</v>
       </c>
       <c r="F17">
-        <v>253.45833333333334</v>
+        <v>173.97833333333335</v>
       </c>
       <c r="G17">
+        <f t="shared" si="2"/>
+        <v>2.7184114583333337E-5</v>
+      </c>
+      <c r="H17">
+        <v>178.333</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="3"/>
+        <v>2.7864531250000001E-5</v>
+      </c>
+      <c r="J17">
         <f t="shared" si="0"/>
         <v>3.283203125E-6</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K17">
+        <f t="shared" si="1"/>
+        <v>3.9602864583333335E-6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -900,14 +1216,29 @@
         <v>5.571621734288863</v>
       </c>
       <c r="F18">
-        <v>267.10416666666669</v>
+        <v>185.6371666666667</v>
       </c>
       <c r="G18">
+        <f t="shared" si="2"/>
+        <v>2.9005807291666673E-5</v>
+      </c>
+      <c r="H18">
+        <v>194.13766666666663</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="3"/>
+        <v>3.0334010416666662E-5</v>
+      </c>
+      <c r="J18">
         <f t="shared" si="0"/>
         <v>3.5611979166666661E-6</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K18">
+        <f t="shared" si="1"/>
+        <v>4.1735026041666669E-6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -924,14 +1255,29 @@
         <v>4.6887498333777664</v>
       </c>
       <c r="F19">
-        <v>261.95833333333331</v>
+        <v>178.50433333333331</v>
       </c>
       <c r="G19">
+        <f t="shared" si="2"/>
+        <v>2.7891302083333328E-5</v>
+      </c>
+      <c r="H19">
+        <v>189.58816666666667</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="3"/>
+        <v>2.9623151041666666E-5</v>
+      </c>
+      <c r="J19">
         <f t="shared" si="0"/>
         <v>3.5211588541666663E-6</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K19">
+        <f t="shared" si="1"/>
+        <v>4.0930989583333334E-6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -948,14 +1294,29 @@
         <v>12.297738613257319</v>
       </c>
       <c r="F20">
-        <v>275.29166666666669</v>
+        <v>189.85066666666668</v>
       </c>
       <c r="G20">
+        <f t="shared" si="2"/>
+        <v>2.966416666666667E-5</v>
+      </c>
+      <c r="H20">
+        <v>190.28866666666664</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="3"/>
+        <v>2.9732604166666663E-5</v>
+      </c>
+      <c r="J20">
         <f t="shared" si="0"/>
         <v>3.5631510416666664E-6</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K20">
+        <f t="shared" si="1"/>
+        <v>4.301432291666667E-6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -972,14 +1333,29 @@
         <v>7.8203294101548915</v>
       </c>
       <c r="F21">
-        <v>261.91666666666669</v>
+        <v>174.48866666666669</v>
       </c>
       <c r="G21">
+        <f t="shared" si="2"/>
+        <v>2.7263854166666671E-5</v>
+      </c>
+      <c r="H21">
+        <v>182.13499999999996</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="3"/>
+        <v>2.8458593749999993E-5</v>
+      </c>
+      <c r="J21">
         <f t="shared" si="0"/>
         <v>3.4667968749999994E-6</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K21">
+        <f t="shared" si="1"/>
+        <v>4.0924479166666672E-6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -996,14 +1372,29 @@
         <v>2.2847433298585877</v>
       </c>
       <c r="F22">
-        <v>278.58333333333331</v>
+        <v>189.16833333333329</v>
       </c>
       <c r="G22">
+        <f t="shared" si="2"/>
+        <v>2.9557552083333326E-5</v>
+      </c>
+      <c r="H22">
+        <v>179.96049999999997</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="3"/>
+        <v>2.8118828124999995E-5</v>
+      </c>
+      <c r="J22">
         <f t="shared" si="0"/>
         <v>3.4638671874999994E-6</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K22">
+        <f t="shared" si="1"/>
+        <v>4.3528645833333331E-6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1020,14 +1411,29 @@
         <v>1.6610582721064784</v>
       </c>
       <c r="F23">
-        <v>271.95833333333331</v>
+        <v>180.55633333333333</v>
       </c>
       <c r="G23">
+        <f t="shared" si="2"/>
+        <v>2.8211927083333331E-5</v>
+      </c>
+      <c r="H23">
+        <v>167.911</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="3"/>
+        <v>2.6236093749999999E-5</v>
+      </c>
+      <c r="J23">
         <f t="shared" si="0"/>
         <v>3.3066406250000001E-6</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K23">
+        <f t="shared" si="1"/>
+        <v>4.2493489583333329E-6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1044,14 +1450,29 @@
         <v>4.4821695360617513</v>
       </c>
       <c r="F24">
-        <v>271.97916666666663</v>
+        <v>178.59016666666662</v>
       </c>
       <c r="G24">
+        <f t="shared" si="2"/>
+        <v>2.790471354166666E-5</v>
+      </c>
+      <c r="H24">
+        <v>170.34066666666664</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="3"/>
+        <v>2.6615729166666661E-5</v>
+      </c>
+      <c r="J24">
         <f t="shared" si="0"/>
         <v>3.3756510416666661E-6</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K24">
+        <f t="shared" si="1"/>
+        <v>4.249674479166666E-6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1068,11 +1489,26 @@
         <v>6.6922685491044982</v>
       </c>
       <c r="F25">
-        <v>268.66666666666663</v>
+        <v>173.29066666666662</v>
       </c>
       <c r="G25">
+        <f t="shared" si="2"/>
+        <v>2.7076666666666661E-5</v>
+      </c>
+      <c r="H25">
+        <v>165.81199999999995</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="3"/>
+        <v>2.5908124999999992E-5</v>
+      </c>
+      <c r="J25">
         <f t="shared" si="0"/>
         <v>3.3359374999999993E-6</v>
+      </c>
+      <c r="K25">
+        <f t="shared" si="1"/>
+        <v>4.1979166666666659E-6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>